<commit_message>
Updated Product/Sprint1 Backlogs. Added use case diagram. Added Sprint1 use case scenarios. Updated README.
</commit_message>
<xml_diff>
--- a/sprints/Product Backlog.xlsx
+++ b/sprints/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Corley\git\SE2-project-repos-sample\sprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twhal\git\UWG-SE2-Spring20-Group4\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EC7C4E-5288-43E2-BCCD-AFE8A3B4E981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915B4FED-DE88-4DE0-B635-18B15BC26951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39780" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Priority</t>
   </si>
@@ -39,20 +39,119 @@
     <t>Why</t>
   </si>
   <si>
-    <t>As a…</t>
-  </si>
-  <si>
-    <t>I want…</t>
-  </si>
-  <si>
-    <t>So that…</t>
+    <t>user</t>
+  </si>
+  <si>
+    <t>to put a game on a watchlist</t>
+  </si>
+  <si>
+    <t>I can view the price of the game</t>
+  </si>
+  <si>
+    <t>to remove games from my watchlist</t>
+  </si>
+  <si>
+    <t>I can remove games that I am no longer tracking</t>
+  </si>
+  <si>
+    <t>to browse the steam library by entering the name of a game</t>
+  </si>
+  <si>
+    <t>I can find the games that I want on my watchlist</t>
+  </si>
+  <si>
+    <t>to check my notifications in app</t>
+  </si>
+  <si>
+    <t>I don't have to exit the app to view notifications if I don't want to</t>
+  </si>
+  <si>
+    <t>specify "cutoff" for item on watchlist</t>
+  </si>
+  <si>
+    <t>I can get notifications when a game dips below a price point.</t>
+  </si>
+  <si>
+    <t>to be notified by email when notification criteria is met</t>
+  </si>
+  <si>
+    <t>I can purchase the game at a good price</t>
+  </si>
+  <si>
+    <t>to be able to edit my watchlist</t>
+  </si>
+  <si>
+    <t>I can reevaluate the price threshold that I am willing to buy the game at.</t>
+  </si>
+  <si>
+    <t>a link to purchase the game in my notifications</t>
+  </si>
+  <si>
+    <t>I can quickly purchase the game as soon as I get a notification</t>
+  </si>
+  <si>
+    <t>link my Steam account to SteamScout</t>
+  </si>
+  <si>
+    <t>I can transfer my watch list between devices by signing in</t>
+  </si>
+  <si>
+    <t>have a search history to view games that I have added to my list in the past.</t>
+  </si>
+  <si>
+    <t>I can easily find games that I have added to my watch list in the past</t>
+  </si>
+  <si>
+    <t>sort my watchlist by sorting factors such as alphabetical order, rating, price, etc.</t>
+  </si>
+  <si>
+    <t>I can see games that are similar.</t>
+  </si>
+  <si>
+    <t>to search for games by other factors such as genre</t>
+  </si>
+  <si>
+    <t>I can find a game I want even if I don't remember the name</t>
+  </si>
+  <si>
+    <t>recieve relevant results despite a spelling mistake</t>
+  </si>
+  <si>
+    <t>I can find a game if I mispress a key</t>
+  </si>
+  <si>
+    <t>the textfields to autopredict what I am typing</t>
+  </si>
+  <si>
+    <t>I don't have to type so much.</t>
+  </si>
+  <si>
+    <t>to be able to share my watchlist with others</t>
+  </si>
+  <si>
+    <t>I can share my watchlist with others</t>
+  </si>
+  <si>
+    <t>for games on my watchlist to be automatically removed if I buy the game</t>
+  </si>
+  <si>
+    <t>I don't continue getting notifications for a game that I already have</t>
+  </si>
+  <si>
+    <t>to import my wishlist from steam into my watchlist</t>
+  </si>
+  <si>
+    <t>I don't have to manually add games from my wishlist to my watchlist</t>
+  </si>
+  <si>
+    <t>Decided to bump this to second sprint. It makes more sense to tie this in with the server functionality where all of the data is stored, but we have not set up the server yet.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,8 +159,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,12 +181,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,13 +200,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,20 +516,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="3" max="3" width="76.28515625" customWidth="1"/>
+    <col min="4" max="4" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -397,21 +543,249 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>